<commit_message>
add files 12 sept
</commit_message>
<xml_diff>
--- a/Evaluation_Results/Final_TestFiles_3rdSeptember_FewShotTest_Broad/ner_evaluation_results_Llama-3.1-8B-Instruct_3_shot.xlsx
+++ b/Evaluation_Results/Final_TestFiles_3rdSeptember_FewShotTest_Broad/ner_evaluation_results_Llama-3.1-8B-Instruct_3_shot.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,13 +17,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +45,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:X2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -422,25 +434,206 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Model</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Examples</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>OtherMetrics...</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Time (s)</t>
-        </is>
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Model Name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Exact Precision (Micro Avg)</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Exact Recall (Micro Avg)</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Exact F1 Score (Micro Avg)</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Exact Precision (Macro Avg)</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Exact Recall (Macro Avg)</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Exact F1 Score (Macro Avg)</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Exact Precision (Weighted Avg)</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Exact Recall (Weighted Avg)</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Exact F1 Score (Weighted Avg)</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Partial Precision</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Partial Recall</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Partial F1 Score</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Partial TP</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Partial FP</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Partial FN</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Support</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Accuracy</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Result Link</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>Stats Link</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>No of GPU Used</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>Power Consumption</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>09/11/2025</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Llama-3.1-8B-Instruct</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>0.3902439024390244</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.2730375426621161</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.321285140562249</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.2482302011713776</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.1229980723685647</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.1494622268994377</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.5222522642317864</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.2730375426621161</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.3377222915882462</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0.4876847290640394</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0.339041095890411</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="O2" t="n">
+        <v>99</v>
+      </c>
+      <c r="P2" t="n">
+        <v>104</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>193</v>
+      </c>
+      <c r="R2" t="n">
+        <v>293</v>
+      </c>
+      <c r="S2" t="n">
+        <v>0.9476213951195465</v>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>/home/s27mhusa_hpc/Master-Thesis/Evaluation_Results/Final_TestFiles_3rdSeptember_FewShotTest_Broad/ner_evaluation_results_Llama-3.1-8B-Instruct_3_shot.txt</t>
+        </is>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>/home/s27mhusa_hpc/Master-Thesis/Evaluation_Results/Final_TestFiles_3rdSeptember_FewShotTest_Broad/Stats/ner_evaluation_stats_Llama-3.1-8B-Instruct_3_shot.txt</t>
+        </is>
+      </c>
+      <c r="V2" t="inlineStr">
+        <is>
+          <t>4 MLGPU</t>
+        </is>
+      </c>
+      <c r="W2" t="inlineStr">
+        <is>
+          <t>0.014 kWh</t>
+        </is>
+      </c>
+      <c r="X2" t="n">
+        <v>562</v>
       </c>
     </row>
   </sheetData>

</xml_diff>